<commit_message>
Hasta Insertar Parcela OK
</commit_message>
<xml_diff>
--- a/Documentacion APPs/PARAMETROS - CLASES.xlsx
+++ b/Documentacion APPs/PARAMETROS - CLASES.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\sa\sistema-sa\Documentacion APPs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\sa\sistema\Documentacion APPs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="94">
   <si>
     <t>SOLTERO</t>
   </si>
@@ -303,6 +303,12 @@
   </si>
   <si>
     <t>Fecha de Incorporacion</t>
+  </si>
+  <si>
+    <t>PARCELA</t>
+  </si>
+  <si>
+    <t>.:::.PARCELA.:::.</t>
   </si>
 </sst>
 </file>
@@ -718,8 +724,8 @@
   <dimension ref="A1:J311"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E51" sqref="E51"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1754,12 +1760,24 @@
       </c>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
-      <c r="G56" s="2"/>
+      <c r="B56" s="3">
+        <v>0</v>
+      </c>
+      <c r="C56" s="3">
+        <v>2006</v>
+      </c>
+      <c r="D56" s="3">
+        <v>10</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G56" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="58" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B58"/>

</xml_diff>

<commit_message>
Hasta  Insertar en Cuenta Corriente
</commit_message>
<xml_diff>
--- a/Documentacion APPs/PARAMETROS - CLASES.xlsx
+++ b/Documentacion APPs/PARAMETROS - CLASES.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Parametros Finales" sheetId="8" r:id="rId1"/>
     <sheet name="nPerTipo-Persona" sheetId="9" r:id="rId2"/>
     <sheet name="nPerDocTipo -PerDocumeto" sheetId="10" r:id="rId3"/>
     <sheet name="nPerRelTipo-PerRelacion" sheetId="11" r:id="rId4"/>
+    <sheet name="CtaCteEstado" sheetId="12" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="135">
   <si>
     <t>SOLTERO</t>
   </si>
@@ -417,6 +418,21 @@
   </si>
   <si>
     <t>General</t>
+  </si>
+  <si>
+    <t>CtaCteEstado</t>
+  </si>
+  <si>
+    <t>Cuenta Corriente</t>
+  </si>
+  <si>
+    <t>Eliminada</t>
+  </si>
+  <si>
+    <t>Pagada</t>
+  </si>
+  <si>
+    <t>Por Pagar</t>
   </si>
 </sst>
 </file>
@@ -834,7 +850,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J328"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F77" sqref="F77"/>
     </sheetView>
@@ -3063,4 +3079,54 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>